<commit_message>
edits to tb/hiv code to work with new symptom manager
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_HIV.xlsx
+++ b/resources/ResourceFile_HIV.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8310" yWindow="0" windowWidth="14835" windowHeight="9360" tabRatio="723" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="8310" yWindow="0" windowWidth="14835" windowHeight="9360" tabRatio="723"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="26" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="120">
   <si>
     <t>Age</t>
   </si>
@@ -87,12 +87,6 @@
     <t>Initial_state350</t>
   </si>
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Value1</t>
-  </si>
-  <si>
     <t>Value2</t>
   </si>
   <si>
@@ -198,12 +192,6 @@
     <t>vls_child</t>
   </si>
   <si>
-    <t>testing_coverage_male_2010</t>
-  </si>
-  <si>
-    <t>testing_coverage_female_2010</t>
-  </si>
-  <si>
     <t>time_months</t>
   </si>
   <si>
@@ -321,9 +309,6 @@
     <t>monthly_prob_mtct_bf_treated</t>
   </si>
   <si>
-    <t>prop_muslim</t>
-  </si>
-  <si>
     <t>probability_infection</t>
   </si>
   <si>
@@ -406,6 +391,15 @@
   </si>
   <si>
     <t>hv_behav_mod</t>
+  </si>
+  <si>
+    <t>parameter_name</t>
+  </si>
+  <si>
+    <t>testing_coverage_male</t>
+  </si>
+  <si>
+    <t>testing_coverage_female</t>
   </si>
 </sst>
 </file>
@@ -774,11 +768,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -788,115 +782,115 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>0.106</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>2.0824498404409902E-2</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>118</v>
       </c>
       <c r="B4">
         <v>0.50900000000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="B5">
         <v>0.71599999999999997</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>0.89700000000000002</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7">
         <v>0.92100000000000004</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>0.57899999999999996</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>1.08</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,7 +901,7 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -918,7 +912,7 @@
         <v>2.7</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,67 +923,67 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14">
         <v>0.22</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>0.3</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B17">
         <v>0.01</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>6.8999999999999999E-3</v>
@@ -997,7 +991,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20">
         <f>1/5.5</f>
@@ -1006,7 +1000,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -1014,18 +1008,18 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>0.4</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>0.75</v>
@@ -1033,7 +1027,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1041,183 +1035,183 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B25">
         <v>0.52</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B26">
         <v>0.96</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B27">
         <v>1.18</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B28">
         <v>1.19</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B29">
         <v>1.56</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B30">
         <v>1.43</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B31">
         <v>2.15</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B32">
         <v>3.75</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B33">
         <v>5.88</v>
       </c>
       <c r="D33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B34">
         <v>7.57</v>
       </c>
       <c r="D34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B35">
         <v>7.93</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B36">
         <v>6.72</v>
       </c>
       <c r="D36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B37">
         <v>7.9</v>
       </c>
       <c r="D37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B38">
         <v>1.18</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B39">
         <v>1.1499999999999999</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1225,7 +1219,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1233,7 +1227,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1241,7 +1235,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1249,29 +1243,21 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B45">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B46">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47">
         <v>0.31</v>
       </c>
-      <c r="F47" t="s">
-        <v>99</v>
+      <c r="F46" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1446,13 +1432,13 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1520,12 +1506,12 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2">
         <v>21.7</v>
@@ -1533,7 +1519,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>22.2</v>
@@ -1541,7 +1527,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4">
         <v>18.3</v>
@@ -1549,7 +1535,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>22.5</v>
@@ -1557,7 +1543,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>21.7</v>
@@ -1589,25 +1575,25 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>115</v>
-      </c>
-      <c r="D1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,57 +1904,57 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1991,10 +1977,10 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2281,15 +2267,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2">
         <f>LOG(2,2.7182818)/3.25</f>
@@ -2302,7 +2288,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B3">
         <f>LOG(2,2.7182818)/6.2</f>
@@ -2315,7 +2301,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B4">
         <f>LOG(2,2.7182818)/12</f>
@@ -2328,7 +2314,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5">
         <f>LOG(2,2.7182818)/11.4</f>
@@ -2341,7 +2327,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <f>LOG(2,2.7182818)/37.2</f>
@@ -2372,10 +2358,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2634,22 +2620,22 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2663,7 +2649,7 @@
         <v>0.23</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>3637076</v>
@@ -2726,7 +2712,7 @@
         <v>0.18</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>3995699</v>
@@ -2770,7 +2756,7 @@
         <v>0.27900000000000003</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>4263253</v>
@@ -3283,10 +3269,10 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
edits to hiv logger and resourceFile
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_HIV.xlsx
+++ b/resources/ResourceFile_HIV.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8310" yWindow="0" windowWidth="14835" windowHeight="9360" tabRatio="723"/>
+    <workbookView xWindow="8310" yWindow="0" windowWidth="14835" windowHeight="9360" tabRatio="723" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="26" r:id="rId1"/>
     <sheet name="circumcision_dhs2010" sheetId="38" r:id="rId2"/>
-    <sheet name="unaids_estimates" sheetId="39" r:id="rId3"/>
-    <sheet name="IPTdistricts" sheetId="37" r:id="rId4"/>
-    <sheet name="timeSinceInf2010" sheetId="36" r:id="rId5"/>
-    <sheet name="details_rates" sheetId="35" r:id="rId6"/>
-    <sheet name="VL_monitoring" sheetId="33" r:id="rId7"/>
-    <sheet name="circumcision" sheetId="30" r:id="rId8"/>
-    <sheet name="incidence_calibration" sheetId="31" r:id="rId9"/>
-    <sheet name="Initial_state_probs" sheetId="24" r:id="rId10"/>
-    <sheet name="fsw" sheetId="29" r:id="rId11"/>
+    <sheet name="aids_info" sheetId="39" r:id="rId3"/>
+    <sheet name="unaids" sheetId="40" r:id="rId4"/>
+    <sheet name="IPTdistricts" sheetId="37" r:id="rId5"/>
+    <sheet name="timeSinceInf2010" sheetId="36" r:id="rId6"/>
+    <sheet name="details_rates" sheetId="35" r:id="rId7"/>
+    <sheet name="VL_monitoring" sheetId="33" r:id="rId8"/>
+    <sheet name="circumcision" sheetId="30" r:id="rId9"/>
+    <sheet name="incidence_calibration" sheetId="31" r:id="rId10"/>
+    <sheet name="Initial_state_probs" sheetId="24" r:id="rId11"/>
+    <sheet name="fsw" sheetId="29" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="145">
   <si>
     <t>Age</t>
   </si>
@@ -412,6 +413,69 @@
   </si>
   <si>
     <t>treatment_prob</t>
+  </si>
+  <si>
+    <t>prev_15_49</t>
+  </si>
+  <si>
+    <t>inc_15_49_per1000</t>
+  </si>
+  <si>
+    <t>inc_15_49_per1000lower</t>
+  </si>
+  <si>
+    <t>inc_15_49_per1000upper</t>
+  </si>
+  <si>
+    <t>inc_15_49_percent_lower</t>
+  </si>
+  <si>
+    <t>inc_15_49_percent_upper</t>
+  </si>
+  <si>
+    <t>prev_15_49_lower</t>
+  </si>
+  <si>
+    <t>prev_15_49_upper</t>
+  </si>
+  <si>
+    <t>number_deaths_15plus</t>
+  </si>
+  <si>
+    <t>number_deaths_15plus_lower</t>
+  </si>
+  <si>
+    <t>number_deaths_15plus_upper</t>
+  </si>
+  <si>
+    <t>mort_rate</t>
+  </si>
+  <si>
+    <t>mort_rate_lower</t>
+  </si>
+  <si>
+    <t>mort_rate_upper</t>
+  </si>
+  <si>
+    <t>percent15plus_on_art</t>
+  </si>
+  <si>
+    <t>percent15plus_on_art_lower</t>
+  </si>
+  <si>
+    <t>percent15plus_on_art_upper</t>
+  </si>
+  <si>
+    <t>inc_15_49_percent</t>
+  </si>
+  <si>
+    <t>mort_rate100k</t>
+  </si>
+  <si>
+    <t>mort_rate100k_lower</t>
+  </si>
+  <si>
+    <t>mort_rate100k_upper</t>
   </si>
 </sst>
 </file>
@@ -783,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
@@ -1296,6 +1360,146 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2009</v>
+      </c>
+      <c r="B2">
+        <v>44156</v>
+      </c>
+      <c r="C2">
+        <v>17808</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2010</v>
+      </c>
+      <c r="B3">
+        <v>42441</v>
+      </c>
+      <c r="C3">
+        <v>17260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4">
+        <v>40671</v>
+      </c>
+      <c r="C4">
+        <v>13781</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2012</v>
+      </c>
+      <c r="B5">
+        <v>38359</v>
+      </c>
+      <c r="C5">
+        <v>11343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2013</v>
+      </c>
+      <c r="B6">
+        <v>36155</v>
+      </c>
+      <c r="C6">
+        <v>9413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2014</v>
+      </c>
+      <c r="B7">
+        <v>34550</v>
+      </c>
+      <c r="C7">
+        <v>8190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2015</v>
+      </c>
+      <c r="B8">
+        <v>32933</v>
+      </c>
+      <c r="C8">
+        <v>6009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2016</v>
+      </c>
+      <c r="B9">
+        <v>31636</v>
+      </c>
+      <c r="C9">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2017</v>
+      </c>
+      <c r="B10">
+        <v>29898</v>
+      </c>
+      <c r="C10">
+        <v>3790</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2018</v>
+      </c>
+      <c r="B11">
+        <v>29868</v>
+      </c>
+      <c r="C11">
+        <v>3037</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1440,7 +1644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1585,415 +1789,862 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="4.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="14.625" customWidth="1"/>
+    <col min="21" max="21" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="H1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="I1" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="J1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" t="s">
+        <v>134</v>
+      </c>
+      <c r="O1" t="s">
+        <v>135</v>
+      </c>
+      <c r="P1" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R1" t="s">
+        <v>142</v>
+      </c>
+      <c r="S1" t="s">
+        <v>143</v>
+      </c>
+      <c r="T1" t="s">
+        <v>144</v>
+      </c>
+      <c r="U1" t="s">
+        <v>138</v>
+      </c>
+      <c r="V1" t="s">
+        <v>139</v>
+      </c>
+      <c r="W1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
-      <c r="B2" s="3">
-        <v>0.62</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0.27005271462432529</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0.1036</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2.0824498404409902E-2</v>
+      <c r="B2">
+        <v>7.1</v>
+      </c>
+      <c r="C2">
+        <v>6.6</v>
+      </c>
+      <c r="D2">
+        <v>7.52</v>
+      </c>
+      <c r="E2">
+        <f>B2/10</f>
+        <v>0.71</v>
       </c>
       <c r="F2">
-        <v>4.15939940755176</v>
+        <f t="shared" ref="F2:G2" si="0">C2/10</f>
+        <v>0.65999999999999992</v>
       </c>
       <c r="G2">
-        <v>28.3</v>
-      </c>
-      <c r="H2">
-        <v>13.93</v>
-      </c>
-      <c r="I2">
-        <v>4.15939940755176</v>
-      </c>
-      <c r="J2" s="4">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10.6</v>
+      </c>
+      <c r="I2" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J2" s="3">
+        <v>11.7</v>
+      </c>
+      <c r="K2" s="4">
         <v>7927106</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L2" s="3">
+        <v>18000</v>
+      </c>
+      <c r="M2" s="3">
+        <v>16000</v>
+      </c>
+      <c r="N2" s="3">
+        <v>22000</v>
+      </c>
+      <c r="O2">
+        <f>L2/$K2</f>
+        <v>2.2706899592360693E-3</v>
+      </c>
+      <c r="P2">
+        <f>M2/$K2</f>
+        <v>2.0183910748765061E-3</v>
+      </c>
+      <c r="Q2">
+        <f>N2/$K2</f>
+        <v>2.7752877279551957E-3</v>
+      </c>
+      <c r="R2">
+        <f>O2*100000</f>
+        <v>227.06899592360693</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ref="S2:T2" si="1">P2*100000</f>
+        <v>201.83910748765061</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="1"/>
+        <v>277.52877279551956</v>
+      </c>
+      <c r="U2">
+        <v>31</v>
+      </c>
+      <c r="V2">
+        <v>27</v>
+      </c>
+      <c r="W2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
-      <c r="B3" s="3">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.21986252002984824</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.1017</v>
-      </c>
-      <c r="E3" s="3">
-        <v>1.9841554773700965E-2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>3.6934633599961044</v>
+      <c r="B3">
+        <v>6.8</v>
+      </c>
+      <c r="C3">
+        <v>6.36</v>
+      </c>
+      <c r="D3">
+        <v>7.26</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="2">B3/10</f>
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="3">C3/10</f>
+        <v>0.63600000000000001</v>
       </c>
       <c r="G3">
-        <v>35.950000000000003</v>
-      </c>
-      <c r="H3">
-        <v>18.07</v>
-      </c>
-      <c r="I3">
-        <v>3.6934633599961044</v>
-      </c>
-      <c r="J3" s="4">
+        <f t="shared" ref="G3:G13" si="4">D3/10</f>
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="H3" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J3" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="K3" s="4">
         <v>8213700</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="3">
+        <v>16000</v>
+      </c>
+      <c r="M3" s="3">
+        <v>14000</v>
+      </c>
+      <c r="N3" s="3">
+        <v>20000</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O10" si="5">L3/$K3</f>
+        <v>1.9479649853293888E-3</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P10" si="6">M3/$K3</f>
+        <v>1.7044693621632151E-3</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q10" si="7">N3/$K3</f>
+        <v>2.4349562316617361E-3</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R13" si="8">O3*100000</f>
+        <v>194.79649853293887</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S13" si="9">P3*100000</f>
+        <v>170.44693621632152</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T13" si="10">Q3*100000</f>
+        <v>243.4956231661736</v>
+      </c>
+      <c r="U3">
+        <v>39</v>
+      </c>
+      <c r="V3">
+        <v>34</v>
+      </c>
+      <c r="W3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
-      <c r="B4" s="3">
-        <v>0.52</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.19227500023343339</v>
-      </c>
-      <c r="D4" s="3">
-        <v>9.9700000000000011E-2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>1.8903657523142881E-2</v>
-      </c>
-      <c r="F4" s="3">
-        <v>3.3337664934731071</v>
+      <c r="B4">
+        <v>6.4</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>6.93</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>0.64</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
       </c>
       <c r="G4">
-        <v>44.11</v>
-      </c>
-      <c r="H4">
-        <v>24.2</v>
-      </c>
-      <c r="I4">
-        <v>3.3337664934731071</v>
-      </c>
-      <c r="J4" s="4">
+        <f t="shared" si="4"/>
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="H4" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="I4" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="K4" s="4">
         <v>8511094</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="3">
+        <v>14000</v>
+      </c>
+      <c r="M4" s="3">
+        <v>12000</v>
+      </c>
+      <c r="N4" s="3">
+        <v>17000</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="5"/>
+        <v>1.6449119231910728E-3</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="6"/>
+        <v>1.4099245055923481E-3</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="7"/>
+        <v>1.9973930495891597E-3</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="8"/>
+        <v>164.49119231910728</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="9"/>
+        <v>140.99245055923481</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="10"/>
+        <v>199.73930495891597</v>
+      </c>
+      <c r="U4">
+        <v>47</v>
+      </c>
+      <c r="V4">
+        <v>41</v>
+      </c>
+      <c r="W4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.47</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.16413302534279467</v>
-      </c>
-      <c r="D5" s="3">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>1.8046946077145277E-2</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2.8166800705201811</v>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>5.57</v>
+      </c>
+      <c r="D5">
+        <v>6.55</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>0.55700000000000005</v>
       </c>
       <c r="G5">
-        <v>49.74</v>
-      </c>
-      <c r="H5">
-        <v>30.51</v>
-      </c>
-      <c r="I5">
-        <v>2.8166800705201811</v>
-      </c>
-      <c r="J5" s="4">
+        <f t="shared" si="4"/>
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I5" s="3">
+        <v>9</v>
+      </c>
+      <c r="J5" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="K5" s="4">
         <v>8819603</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" s="3">
+        <v>12000</v>
+      </c>
+      <c r="M5" s="3">
+        <v>9600</v>
+      </c>
+      <c r="N5" s="3">
+        <v>15000</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>1.3606054603591568E-3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>1.0884843682873254E-3</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="7"/>
+        <v>1.7007568254489458E-3</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="8"/>
+        <v>136.06054603591568</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="9"/>
+        <v>108.84843682873253</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="10"/>
+        <v>170.07568254489459</v>
+      </c>
+      <c r="U5">
+        <v>53</v>
+      </c>
+      <c r="V5">
+        <v>47</v>
+      </c>
+      <c r="W5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
-      <c r="B6" s="3">
-        <v>0.43</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.14595408019679024</v>
-      </c>
-      <c r="D6" s="3">
-        <v>9.6300000000000011E-2</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1.718293716008773E-2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>2.4489049916576788</v>
+      <c r="B6">
+        <v>5.7</v>
+      </c>
+      <c r="C6">
+        <v>5.27</v>
+      </c>
+      <c r="D6">
+        <v>6.17</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>0.52699999999999991</v>
       </c>
       <c r="G6">
-        <v>56.39</v>
-      </c>
-      <c r="H6">
-        <v>34</v>
-      </c>
-      <c r="I6">
-        <v>2.4489049916576788</v>
-      </c>
-      <c r="J6" s="4">
+        <f t="shared" si="4"/>
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J6" s="3">
+        <v>10.9</v>
+      </c>
+      <c r="K6" s="4">
         <v>9137145</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="3">
+        <v>11000</v>
+      </c>
+      <c r="M6" s="3">
+        <v>8700</v>
+      </c>
+      <c r="N6" s="3">
+        <v>13000</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>1.203877141054454E-3</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>9.5215737519761367E-4</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="7"/>
+        <v>1.4227638939734457E-3</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="8"/>
+        <v>120.3877141054454</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="9"/>
+        <v>95.215737519761362</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="10"/>
+        <v>142.27638939734456</v>
+      </c>
+      <c r="U6">
+        <v>58</v>
+      </c>
+      <c r="V6">
+        <v>52</v>
+      </c>
+      <c r="W6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
-      <c r="B7" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.11758890434882779</v>
-      </c>
-      <c r="D7" s="3">
-        <v>9.4600000000000004E-2</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1.6164578832912037E-2</v>
-      </c>
-      <c r="F7" s="3">
-        <v>2.2100662121462746</v>
+      <c r="B7">
+        <v>5.4</v>
+      </c>
+      <c r="C7">
+        <v>4.95</v>
+      </c>
+      <c r="D7">
+        <v>5.86</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>0.54</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>0.495</v>
       </c>
       <c r="G7">
-        <v>60.71</v>
-      </c>
-      <c r="H7">
-        <v>45.33</v>
-      </c>
-      <c r="I7">
-        <v>2.2100662121462746</v>
-      </c>
-      <c r="J7" s="4">
+        <f t="shared" si="4"/>
+        <v>0.58600000000000008</v>
+      </c>
+      <c r="H7" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I7" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J7" s="3">
+        <v>10.7</v>
+      </c>
+      <c r="K7" s="4">
         <v>9461255</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M7" s="3">
+        <v>8300</v>
+      </c>
+      <c r="N7" s="3">
+        <v>13000</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>1.0569422344075918E-3</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>8.772620545583012E-4</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="7"/>
+        <v>1.3740249047298693E-3</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="8"/>
+        <v>105.69422344075919</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="9"/>
+        <v>87.726205455830126</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="10"/>
+        <v>137.40249047298693</v>
+      </c>
+      <c r="U7">
+        <v>62</v>
+      </c>
+      <c r="V7">
+        <v>55</v>
+      </c>
+      <c r="W7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2016</v>
       </c>
-      <c r="B8" s="3">
-        <v>0.37</v>
-      </c>
-      <c r="C8" s="3">
-        <v>9.969591721676839E-2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>9.3000000000000013E-2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1.5147092079585865E-2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>2.0117021463466846</v>
+      <c r="B8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C8">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="D8">
+        <v>5.67</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>0.51</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>0.46100000000000002</v>
       </c>
       <c r="G8">
-        <v>68.7</v>
-      </c>
-      <c r="H8">
-        <v>49.25</v>
-      </c>
-      <c r="I8">
-        <v>2.0117021463466846</v>
-      </c>
-      <c r="J8" s="4">
+        <f t="shared" si="4"/>
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="H8" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="I8" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="J8" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="K8" s="4">
         <v>9791708</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M8" s="3">
+        <v>8400</v>
+      </c>
+      <c r="N8" s="3">
+        <v>13000</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>1.0212722846718878E-3</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>8.578687191243856E-4</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>1.3276539700734539E-3</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="8"/>
+        <v>102.12722846718877</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="9"/>
+        <v>85.786871912438556</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="10"/>
+        <v>132.7653970073454</v>
+      </c>
+      <c r="U8">
+        <v>69</v>
+      </c>
+      <c r="V8">
+        <v>61</v>
+      </c>
+      <c r="W8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2017</v>
       </c>
-      <c r="B9" s="3">
-        <v>0.34</v>
-      </c>
-      <c r="C9" s="3">
-        <v>8.697191076765079E-2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>9.1400000000000009E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1.4176408048018899E-2</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1.8158446288510319</v>
+      <c r="B9">
+        <v>4.7</v>
+      </c>
+      <c r="C9">
+        <v>4.16</v>
+      </c>
+      <c r="D9">
+        <v>5.34</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>0.47000000000000003</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>0.41600000000000004</v>
       </c>
       <c r="G9">
-        <v>68.180000000000007</v>
-      </c>
-      <c r="H9">
-        <v>56.71</v>
-      </c>
-      <c r="I9">
-        <v>1.8158446288510319</v>
-      </c>
-      <c r="J9" s="4">
+        <f t="shared" si="4"/>
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="H9" s="3">
+        <v>9.4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J9" s="3">
+        <v>10.3</v>
+      </c>
+      <c r="K9" s="4">
         <v>10130272</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M9" s="3">
+        <v>8600</v>
+      </c>
+      <c r="N9" s="3">
+        <v>12000</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>9.8714032555098229E-4</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>8.4894067997384477E-4</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="7"/>
+        <v>1.1845683906611787E-3</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="8"/>
+        <v>98.714032555098228</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="9"/>
+        <v>84.894067997384482</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="10"/>
+        <v>118.45683906611788</v>
+      </c>
+      <c r="U9">
+        <v>74</v>
+      </c>
+      <c r="V9">
+        <v>66</v>
+      </c>
+      <c r="W9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="C10" s="3">
-        <v>7.6328011746993149E-2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>8.9700000000000002E-2</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1.3208638299034547E-2</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1.7718707782773453</v>
-      </c>
-      <c r="I10">
-        <v>1.7718707782773453</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="B10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C10">
+        <v>3.77</v>
+      </c>
+      <c r="D10">
+        <v>5.09</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.44000000000000006</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>0.377</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="H10" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="I10" s="3">
+        <v>8</v>
+      </c>
+      <c r="J10" s="3">
+        <v>10</v>
+      </c>
+      <c r="K10" s="4">
         <v>10477062</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M10" s="3">
+        <v>8700</v>
+      </c>
+      <c r="N10" s="3">
+        <v>13000</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>9.5446605164692161E-4</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>8.3038546493282184E-4</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="7"/>
+        <v>1.2408058671409981E-3</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="8"/>
+        <v>95.446605164692158</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="9"/>
+        <v>83.038546493282183</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="10"/>
+        <v>124.08058671409981</v>
+      </c>
+      <c r="U10">
+        <v>79</v>
+      </c>
+      <c r="V10">
+        <v>71</v>
+      </c>
+      <c r="W10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2019</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.31</v>
-      </c>
-      <c r="C11" s="3">
-        <v>6.7746243674404294E-2</v>
-      </c>
-      <c r="D11" s="3">
-        <v>8.8000000000000009E-2</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1.2278762717057625E-2</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1.692746795061145</v>
-      </c>
-      <c r="I11">
-        <v>1.692746795061145</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="4">
         <v>10833280</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2020</v>
       </c>
-      <c r="B12" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="C12" s="3">
-        <v>6.2804411762437076E-2</v>
-      </c>
-      <c r="D12" s="3">
-        <v>8.6400000000000005E-2</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1.142834588735884E-2</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1.5375778398781439</v>
-      </c>
-      <c r="I12">
-        <v>1.5375778398781439</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4">
         <v>11199433</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2021</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="C13" s="3">
-        <v>6.0813696426074822E-2</v>
-      </c>
-      <c r="D13" s="3">
-        <v>8.4700000000000011E-2</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1.067257452542779E-2</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1.3828302536340653</v>
-      </c>
-      <c r="I13">
-        <v>1.3828302536340653</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4">
         <v>11575535</v>
       </c>
+      <c r="L13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2001,6 +2652,425 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.27005271462432529</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.1036</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2.0824498404409902E-2</v>
+      </c>
+      <c r="F2">
+        <v>4.15939940755176</v>
+      </c>
+      <c r="G2">
+        <v>28.3</v>
+      </c>
+      <c r="H2">
+        <v>13.93</v>
+      </c>
+      <c r="I2">
+        <v>4.15939940755176</v>
+      </c>
+      <c r="J2" s="4">
+        <v>7927106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.21986252002984824</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.1017</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.9841554773700965E-2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3.6934633599961044</v>
+      </c>
+      <c r="G3">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="H3">
+        <v>18.07</v>
+      </c>
+      <c r="I3">
+        <v>3.6934633599961044</v>
+      </c>
+      <c r="J3" s="4">
+        <v>8213700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.19227500023343339</v>
+      </c>
+      <c r="D4" s="3">
+        <v>9.9700000000000011E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.8903657523142881E-2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3.3337664934731071</v>
+      </c>
+      <c r="G4">
+        <v>44.11</v>
+      </c>
+      <c r="H4">
+        <v>24.2</v>
+      </c>
+      <c r="I4">
+        <v>3.3337664934731071</v>
+      </c>
+      <c r="J4" s="4">
+        <v>8511094</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.16413302534279467</v>
+      </c>
+      <c r="D5" s="3">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.8046946077145277E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2.8166800705201811</v>
+      </c>
+      <c r="G5">
+        <v>49.74</v>
+      </c>
+      <c r="H5">
+        <v>30.51</v>
+      </c>
+      <c r="I5">
+        <v>2.8166800705201811</v>
+      </c>
+      <c r="J5" s="4">
+        <v>8819603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.14595408019679024</v>
+      </c>
+      <c r="D6" s="3">
+        <v>9.6300000000000011E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.718293716008773E-2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.4489049916576788</v>
+      </c>
+      <c r="G6">
+        <v>56.39</v>
+      </c>
+      <c r="H6">
+        <v>34</v>
+      </c>
+      <c r="I6">
+        <v>2.4489049916576788</v>
+      </c>
+      <c r="J6" s="4">
+        <v>9137145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.11758890434882779</v>
+      </c>
+      <c r="D7" s="3">
+        <v>9.4600000000000004E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.6164578832912037E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.2100662121462746</v>
+      </c>
+      <c r="G7">
+        <v>60.71</v>
+      </c>
+      <c r="H7">
+        <v>45.33</v>
+      </c>
+      <c r="I7">
+        <v>2.2100662121462746</v>
+      </c>
+      <c r="J7" s="4">
+        <v>9461255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9.969591721676839E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>9.3000000000000013E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.5147092079585865E-2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2.0117021463466846</v>
+      </c>
+      <c r="G8">
+        <v>68.7</v>
+      </c>
+      <c r="H8">
+        <v>49.25</v>
+      </c>
+      <c r="I8">
+        <v>2.0117021463466846</v>
+      </c>
+      <c r="J8" s="4">
+        <v>9791708</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8.697191076765079E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>9.1400000000000009E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.4176408048018899E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.8158446288510319</v>
+      </c>
+      <c r="G9">
+        <v>68.180000000000007</v>
+      </c>
+      <c r="H9">
+        <v>56.71</v>
+      </c>
+      <c r="I9">
+        <v>1.8158446288510319</v>
+      </c>
+      <c r="J9" s="4">
+        <v>10130272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7.6328011746993149E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8.9700000000000002E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.3208638299034547E-2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.7718707782773453</v>
+      </c>
+      <c r="I10">
+        <v>1.7718707782773453</v>
+      </c>
+      <c r="J10" s="4">
+        <v>10477062</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="C11" s="3">
+        <v>6.7746243674404294E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>8.8000000000000009E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.2278762717057625E-2</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1.692746795061145</v>
+      </c>
+      <c r="I11">
+        <v>1.692746795061145</v>
+      </c>
+      <c r="J11" s="4">
+        <v>10833280</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C12" s="3">
+        <v>6.2804411762437076E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.142834588735884E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.5375778398781439</v>
+      </c>
+      <c r="I12">
+        <v>1.5375778398781439</v>
+      </c>
+      <c r="J12" s="4">
+        <v>11199433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="C13" s="3">
+        <v>6.0813696426074822E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>8.4700000000000011E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.067257452542779E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1.3828302536340653</v>
+      </c>
+      <c r="I13">
+        <v>1.3828302536340653</v>
+      </c>
+      <c r="J13" s="4">
+        <v>11575535</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
@@ -2073,7 +3143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -2363,7 +3433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2454,7 +3524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -2711,7 +3781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -3359,144 +4429,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2009</v>
-      </c>
-      <c r="B2">
-        <v>44156</v>
-      </c>
-      <c r="C2">
-        <v>17808</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2010</v>
-      </c>
-      <c r="B3">
-        <v>42441</v>
-      </c>
-      <c r="C3">
-        <v>17260</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2011</v>
-      </c>
-      <c r="B4">
-        <v>40671</v>
-      </c>
-      <c r="C4">
-        <v>13781</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2012</v>
-      </c>
-      <c r="B5">
-        <v>38359</v>
-      </c>
-      <c r="C5">
-        <v>11343</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2013</v>
-      </c>
-      <c r="B6">
-        <v>36155</v>
-      </c>
-      <c r="C6">
-        <v>9413</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2014</v>
-      </c>
-      <c r="B7">
-        <v>34550</v>
-      </c>
-      <c r="C7">
-        <v>8190</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2015</v>
-      </c>
-      <c r="B8">
-        <v>32933</v>
-      </c>
-      <c r="C8">
-        <v>6009</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2016</v>
-      </c>
-      <c r="B9">
-        <v>31636</v>
-      </c>
-      <c r="C9">
-        <v>4700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2017</v>
-      </c>
-      <c r="B10">
-        <v>29898</v>
-      </c>
-      <c r="C10">
-        <v>3790</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2018</v>
-      </c>
-      <c r="B11">
-        <v>29868</v>
-      </c>
-      <c r="C11">
-        <v>3037</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>